<commit_message>
Update Lemon Shark leslie matrix
</commit_message>
<xml_diff>
--- a/00_key_resources/leslie matrix lemon sharks.xlsx
+++ b/00_key_resources/leslie matrix lemon sharks.xlsx
@@ -1,35 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlotteboyd/Documents/RESEARCH/WORK IN PROGRESS/d lemon sharks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\00_key_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310C655-D719-B847-A616-94191BF5E54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D628279-C10E-4672-B31E-4B6C244CF15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{D9C3A475-DFFC-3C44-AD51-F6154DA1030C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D9C3A475-DFFC-3C44-AD51-F6154DA1030C}"/>
   </bookViews>
   <sheets>
-    <sheet name="matrix" sheetId="2" r:id="rId1"/>
+    <sheet name="LemonSharkLeslieMatrix" sheetId="2" r:id="rId1"/>
+    <sheet name="WaplesLifeTable" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="A">matrix!$R$8</definedName>
+    <definedName name="A">LemonSharkLeslieMatrix!$R$8</definedName>
     <definedName name="chi">#REF!</definedName>
-    <definedName name="f0" localSheetId="0">matrix!$R$1</definedName>
+    <definedName name="f0" localSheetId="0">LemonSharkLeslieMatrix!$R$1</definedName>
     <definedName name="f0">#REF!</definedName>
-    <definedName name="fx">matrix!$R$12</definedName>
-    <definedName name="N">matrix!$R$7</definedName>
-    <definedName name="p.A">matrix!$R$6</definedName>
+    <definedName name="fx">LemonSharkLeslieMatrix!$R$12</definedName>
+    <definedName name="N">LemonSharkLeslieMatrix!$R$7</definedName>
+    <definedName name="p.A">LemonSharkLeslieMatrix!$R$6</definedName>
     <definedName name="phi">#REF!</definedName>
     <definedName name="rho">#REF!</definedName>
-    <definedName name="s.a" localSheetId="0">matrix!$R$4</definedName>
+    <definedName name="s.a" localSheetId="0">LemonSharkLeslieMatrix!$R$4</definedName>
     <definedName name="s.a">#REF!</definedName>
-    <definedName name="s.c" localSheetId="0">matrix!$R$2</definedName>
+    <definedName name="s.c" localSheetId="0">LemonSharkLeslieMatrix!$R$2</definedName>
     <definedName name="s.c">#REF!</definedName>
-    <definedName name="s.j" localSheetId="0">matrix!$R$3</definedName>
+    <definedName name="s.j" localSheetId="0">LemonSharkLeslieMatrix!$R$3</definedName>
     <definedName name="s.j">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>s.j</t>
   </si>
@@ -149,6 +150,30 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>sx</t>
+  </si>
+  <si>
+    <t>lx</t>
+  </si>
+  <si>
+    <t>Nx</t>
+  </si>
+  <si>
+    <t>bx</t>
+  </si>
+  <si>
+    <t>Nxbx</t>
+  </si>
+  <si>
+    <t>ERRO</t>
+  </si>
+  <si>
+    <t>ERRO is the births per female (bx) divided by the total reproductive output. Here, fecundity is constant across age classes, so each age class has the same ERRO.</t>
   </si>
 </sst>
 </file>
@@ -203,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -217,6 +242,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -536,19 +564,19 @@
   <dimension ref="A1:AB101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.83203125" style="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.875" style="1"/>
+    <col min="19" max="19" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -605,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>f0*M2</f>
         <v>398.32944316561651</v>
@@ -676,7 +704,7 @@
         <v>0.39832944316561653</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A13" si="5">f0*M2</f>
         <v>398.32944316561651</v>
@@ -752,7 +780,7 @@
       </c>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -828,7 +856,7 @@
       </c>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -898,7 +926,7 @@
       </c>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -975,7 +1003,7 @@
       </c>
       <c r="W6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1052,7 +1080,7 @@
       </c>
       <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1128,7 +1156,7 @@
       </c>
       <c r="W8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1199,7 +1227,7 @@
       </c>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1272,7 +1300,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1343,7 +1371,7 @@
       <c r="W11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1412,7 +1440,7 @@
         <v>0.1234567901234567</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1481,7 +1509,7 @@
         <v>0.11111111111111104</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f t="shared" ref="A14:A17" si="16">f0*M13</f>
         <v>398.32944316561651</v>
@@ -1550,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" si="16"/>
         <v>398.32944316561651</v>
@@ -1612,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f t="shared" si="16"/>
         <v>398.32944316561651</v>
@@ -1675,7 +1703,7 @@
       </c>
       <c r="Q16" s="9"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" si="16"/>
         <v>398.32944316561651</v>
@@ -1737,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1753,7 +1781,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1777,7 +1805,7 @@
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1801,7 +1829,7 @@
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1825,7 +1853,7 @@
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1841,7 +1869,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1857,7 +1885,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1875,7 +1903,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1892,7 +1920,7 @@
       <c r="N25" s="5"/>
       <c r="V25" s="3"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1908,7 +1936,7 @@
       <c r="M26" s="8"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1924,7 +1952,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1942,7 +1970,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1959,7 +1987,7 @@
       <c r="N29" s="5"/>
       <c r="V29" s="3"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1975,7 +2003,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1991,7 +2019,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2009,7 +2037,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2028,7 +2056,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2045,7 +2073,7 @@
       <c r="N34" s="5"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2061,7 +2089,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2077,7 +2105,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2093,7 +2121,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2109,7 +2137,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2127,7 +2155,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2144,7 +2172,7 @@
       <c r="N40" s="5"/>
       <c r="V40" s="3"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2160,7 +2188,7 @@
       <c r="M41" s="8"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2176,7 +2204,7 @@
       <c r="M42" s="8"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2192,7 +2220,7 @@
       <c r="M43" s="8"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2208,7 +2236,7 @@
       <c r="M44" s="8"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2224,7 +2252,7 @@
       <c r="M45" s="8"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2242,7 +2270,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2261,7 +2289,7 @@
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2278,7 +2306,7 @@
       <c r="N48" s="5"/>
       <c r="V48" s="3"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2294,7 +2322,7 @@
       <c r="M49" s="8"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2310,7 +2338,7 @@
       <c r="M50" s="8"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2326,7 +2354,7 @@
       <c r="M51" s="8"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2342,7 +2370,7 @@
       <c r="M52" s="8"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2358,7 +2386,7 @@
       <c r="M53" s="8"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2374,7 +2402,7 @@
       <c r="M54" s="8"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2390,7 +2418,7 @@
       <c r="M55" s="8"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2406,7 +2434,7 @@
       <c r="M56" s="8"/>
       <c r="N56" s="5"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2422,7 +2450,7 @@
       <c r="M57" s="8"/>
       <c r="N57" s="5"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2438,7 +2466,7 @@
       <c r="M58" s="8"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2454,7 +2482,7 @@
       <c r="M59" s="8"/>
       <c r="N59" s="5"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2470,7 +2498,7 @@
       <c r="M60" s="8"/>
       <c r="N60" s="5"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2486,7 +2514,7 @@
       <c r="M61" s="8"/>
       <c r="N61" s="5"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2502,7 +2530,7 @@
       <c r="M62" s="8"/>
       <c r="N62" s="5"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -2518,7 +2546,7 @@
       <c r="M63" s="8"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2534,7 +2562,7 @@
       <c r="M64" s="8"/>
       <c r="N64" s="5"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -2550,7 +2578,7 @@
       <c r="M65" s="8"/>
       <c r="N65" s="5"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2566,7 +2594,7 @@
       <c r="M66" s="8"/>
       <c r="N66" s="5"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -2582,7 +2610,7 @@
       <c r="M67" s="8"/>
       <c r="N67" s="5"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2598,7 +2626,7 @@
       <c r="M68" s="8"/>
       <c r="N68" s="5"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2614,7 +2642,7 @@
       <c r="M69" s="8"/>
       <c r="N69" s="5"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2630,7 +2658,7 @@
       <c r="M70" s="8"/>
       <c r="N70" s="5"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2646,7 +2674,7 @@
       <c r="M71" s="8"/>
       <c r="N71" s="5"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2662,7 +2690,7 @@
       <c r="M72" s="8"/>
       <c r="N72" s="5"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2678,7 +2706,7 @@
       <c r="M73" s="8"/>
       <c r="N73" s="5"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2694,7 +2722,7 @@
       <c r="M74" s="8"/>
       <c r="N74" s="5"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2710,7 +2738,7 @@
       <c r="M75" s="8"/>
       <c r="N75" s="5"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -2726,7 +2754,7 @@
       <c r="M76" s="8"/>
       <c r="N76" s="5"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -2742,7 +2770,7 @@
       <c r="M77" s="8"/>
       <c r="N77" s="5"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -2758,7 +2786,7 @@
       <c r="M78" s="8"/>
       <c r="N78" s="5"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -2774,7 +2802,7 @@
       <c r="M79" s="8"/>
       <c r="N79" s="5"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -2790,7 +2818,7 @@
       <c r="M80" s="8"/>
       <c r="N80" s="5"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -2806,7 +2834,7 @@
       <c r="M81" s="8"/>
       <c r="N81" s="5"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -2822,7 +2850,7 @@
       <c r="M82" s="8"/>
       <c r="N82" s="5"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -2838,7 +2866,7 @@
       <c r="M83" s="8"/>
       <c r="N83" s="5"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -2854,7 +2882,7 @@
       <c r="M84" s="8"/>
       <c r="N84" s="5"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2870,7 +2898,7 @@
       <c r="M85" s="8"/>
       <c r="N85" s="5"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2886,7 +2914,7 @@
       <c r="M86" s="8"/>
       <c r="N86" s="5"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -2902,7 +2930,7 @@
       <c r="M87" s="8"/>
       <c r="N87" s="5"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2918,7 +2946,7 @@
       <c r="M88" s="8"/>
       <c r="N88" s="5"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -2934,7 +2962,7 @@
       <c r="M89" s="8"/>
       <c r="N89" s="5"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2950,7 +2978,7 @@
       <c r="M90" s="8"/>
       <c r="N90" s="5"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -2966,7 +2994,7 @@
       <c r="M91" s="8"/>
       <c r="N91" s="5"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -2982,7 +3010,7 @@
       <c r="M92" s="8"/>
       <c r="N92" s="5"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -2998,7 +3026,7 @@
       <c r="M93" s="8"/>
       <c r="N93" s="5"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -3014,7 +3042,7 @@
       <c r="M94" s="8"/>
       <c r="N94" s="5"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -3030,7 +3058,7 @@
       <c r="M95" s="8"/>
       <c r="N95" s="5"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -3046,7 +3074,7 @@
       <c r="M96" s="8"/>
       <c r="N96" s="5"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -3062,7 +3090,7 @@
       <c r="M97" s="8"/>
       <c r="N97" s="5"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -3078,7 +3106,7 @@
       <c r="M98" s="8"/>
       <c r="N98" s="5"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -3094,7 +3122,7 @@
       <c r="M99" s="8"/>
       <c r="N99" s="5"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -3110,7 +3138,7 @@
       <c r="M100" s="8"/>
       <c r="N100" s="5"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="8"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -3133,4 +3161,318 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57290DEC-DCAC-42AC-9583-03780F9F910E}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="83.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <f>E2*D2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="1">
+        <f>C2*B2</f>
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="3">
+        <f>D2*B2</f>
+        <v>700</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F11" si="0">E3*D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.7</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C11" si="1">C3*B3</f>
+        <v>0.48999999999999994</v>
+      </c>
+      <c r="D4" s="3">
+        <f>D3*B3</f>
+        <v>489.99999999999994</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>489.99999999999994</v>
+      </c>
+      <c r="G4">
+        <f>E4/F$12</f>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.34299999999999992</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D11" si="2">D4*B4</f>
+        <v>342.99999999999994</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>342.99999999999994</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G11" si="3">E5/F$12</f>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24009999999999992</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="2"/>
+        <v>240.09999999999994</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>240.09999999999994</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16806999999999994</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>168.06999999999994</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>168.06999999999994</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11764899999999995</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>117.64899999999994</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>117.64899999999994</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.7</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="1"/>
+        <v>8.2354299999999964E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>82.354299999999952</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>82.354299999999952</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7648009999999972E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>57.648009999999964</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>57.648009999999964</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0353606999999979E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>40.353606999999975</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>40.353606999999975</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>6.4969873726184184E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <f>SUM(D2:D11)</f>
+        <v>3239.1749169999998</v>
+      </c>
+      <c r="F12" s="3">
+        <f>SUM(F4:F11)</f>
+        <v>1539.1749169999996</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Connect breeders with total adults in HS|PO model
</commit_message>
<xml_diff>
--- a/00_key_resources/leslie matrix lemon sharks.xlsx
+++ b/00_key_resources/leslie matrix lemon sharks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zeus\Documents\R\working_directory\LemonSharkCKMR\00_key_resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\R\working_directory\LemonSharkCKMR\00_key_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54093B3-233D-4CA1-866D-D88F5C5F543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01183B9C-F26B-42F3-BCC2-6C96B27AA4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{D9C3A475-DFFC-3C44-AD51-F6154DA1030C}"/>
+    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{D9C3A475-DFFC-3C44-AD51-F6154DA1030C}"/>
   </bookViews>
   <sheets>
     <sheet name="LemonSharkLeslieMatrix" sheetId="2" r:id="rId1"/>
@@ -392,7 +392,7 @@
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,12 +420,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -477,10 +471,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -832,16 +826,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.875" style="1"/>
-    <col min="19" max="19" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.8984375" style="1"/>
+    <col min="19" max="19" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -898,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <f>f0*M2</f>
         <v>398.32944316561651</v>
@@ -969,7 +963,7 @@
         <v>0.39832944316561653</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A13" si="5">f0*M2</f>
         <v>398.32944316561651</v>
@@ -1045,7 +1039,7 @@
       </c>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1121,7 +1115,7 @@
       </c>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1191,7 +1185,7 @@
       </c>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1268,7 +1262,7 @@
       </c>
       <c r="W6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1345,7 +1339,7 @@
       </c>
       <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1421,7 +1415,7 @@
       </c>
       <c r="W8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1492,7 +1486,7 @@
       </c>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1565,7 +1559,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1636,7 +1630,7 @@
       <c r="W11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1705,7 +1699,7 @@
         <v>0.1234567901234567</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <f t="shared" si="5"/>
         <v>398.32944316561651</v>
@@ -1774,7 +1768,7 @@
         <v>0.11111111111111104</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <f t="shared" ref="A14:A17" si="16">f0*M13</f>
         <v>398.32944316561651</v>
@@ -1843,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <f t="shared" si="16"/>
         <v>398.32944316561651</v>
@@ -1905,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <f t="shared" si="16"/>
         <v>398.32944316561651</v>
@@ -1968,7 +1962,7 @@
       </c>
       <c r="Q16" s="9"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <f t="shared" si="16"/>
         <v>398.32944316561651</v>
@@ -2030,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2046,7 +2040,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2070,7 +2064,7 @@
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2094,7 +2088,7 @@
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2118,7 +2112,7 @@
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2134,7 +2128,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2150,7 +2144,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2168,7 +2162,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2185,7 +2179,7 @@
       <c r="N25" s="5"/>
       <c r="V25" s="3"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2201,7 +2195,7 @@
       <c r="M26" s="8"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2217,7 +2211,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2235,7 +2229,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2252,7 +2246,7 @@
       <c r="N29" s="5"/>
       <c r="V29" s="3"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2268,7 +2262,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2284,7 +2278,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2302,7 +2296,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2321,7 +2315,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2338,7 +2332,7 @@
       <c r="N34" s="5"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2354,7 +2348,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2370,7 +2364,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2386,7 +2380,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2402,7 +2396,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2420,7 +2414,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2437,7 +2431,7 @@
       <c r="N40" s="5"/>
       <c r="V40" s="3"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2453,7 +2447,7 @@
       <c r="M41" s="8"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2469,7 +2463,7 @@
       <c r="M42" s="8"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2485,7 +2479,7 @@
       <c r="M43" s="8"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2501,7 +2495,7 @@
       <c r="M44" s="8"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2517,7 +2511,7 @@
       <c r="M45" s="8"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2535,7 +2529,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2554,7 +2548,7 @@
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2571,7 +2565,7 @@
       <c r="N48" s="5"/>
       <c r="V48" s="3"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2587,7 +2581,7 @@
       <c r="M49" s="8"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2603,7 +2597,7 @@
       <c r="M50" s="8"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2619,7 +2613,7 @@
       <c r="M51" s="8"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2635,7 +2629,7 @@
       <c r="M52" s="8"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2651,7 +2645,7 @@
       <c r="M53" s="8"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2667,7 +2661,7 @@
       <c r="M54" s="8"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2683,7 +2677,7 @@
       <c r="M55" s="8"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2699,7 +2693,7 @@
       <c r="M56" s="8"/>
       <c r="N56" s="5"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2715,7 +2709,7 @@
       <c r="M57" s="8"/>
       <c r="N57" s="5"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2731,7 +2725,7 @@
       <c r="M58" s="8"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="8"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2747,7 +2741,7 @@
       <c r="M59" s="8"/>
       <c r="N59" s="5"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2763,7 +2757,7 @@
       <c r="M60" s="8"/>
       <c r="N60" s="5"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2779,7 +2773,7 @@
       <c r="M61" s="8"/>
       <c r="N61" s="5"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2795,7 +2789,7 @@
       <c r="M62" s="8"/>
       <c r="N62" s="5"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -2811,7 +2805,7 @@
       <c r="M63" s="8"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2827,7 +2821,7 @@
       <c r="M64" s="8"/>
       <c r="N64" s="5"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -2843,7 +2837,7 @@
       <c r="M65" s="8"/>
       <c r="N65" s="5"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2859,7 +2853,7 @@
       <c r="M66" s="8"/>
       <c r="N66" s="5"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -2875,7 +2869,7 @@
       <c r="M67" s="8"/>
       <c r="N67" s="5"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="8"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2891,7 +2885,7 @@
       <c r="M68" s="8"/>
       <c r="N68" s="5"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2907,7 +2901,7 @@
       <c r="M69" s="8"/>
       <c r="N69" s="5"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2923,7 +2917,7 @@
       <c r="M70" s="8"/>
       <c r="N70" s="5"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2939,7 +2933,7 @@
       <c r="M71" s="8"/>
       <c r="N71" s="5"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2955,7 +2949,7 @@
       <c r="M72" s="8"/>
       <c r="N72" s="5"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2971,7 +2965,7 @@
       <c r="M73" s="8"/>
       <c r="N73" s="5"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2987,7 +2981,7 @@
       <c r="M74" s="8"/>
       <c r="N74" s="5"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="8"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -3003,7 +2997,7 @@
       <c r="M75" s="8"/>
       <c r="N75" s="5"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="8"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -3019,7 +3013,7 @@
       <c r="M76" s="8"/>
       <c r="N76" s="5"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="8"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -3035,7 +3029,7 @@
       <c r="M77" s="8"/>
       <c r="N77" s="5"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="8"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -3051,7 +3045,7 @@
       <c r="M78" s="8"/>
       <c r="N78" s="5"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -3067,7 +3061,7 @@
       <c r="M79" s="8"/>
       <c r="N79" s="5"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -3083,7 +3077,7 @@
       <c r="M80" s="8"/>
       <c r="N80" s="5"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -3099,7 +3093,7 @@
       <c r="M81" s="8"/>
       <c r="N81" s="5"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="8"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -3115,7 +3109,7 @@
       <c r="M82" s="8"/>
       <c r="N82" s="5"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="8"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -3131,7 +3125,7 @@
       <c r="M83" s="8"/>
       <c r="N83" s="5"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -3147,7 +3141,7 @@
       <c r="M84" s="8"/>
       <c r="N84" s="5"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -3163,7 +3157,7 @@
       <c r="M85" s="8"/>
       <c r="N85" s="5"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="8"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -3179,7 +3173,7 @@
       <c r="M86" s="8"/>
       <c r="N86" s="5"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -3195,7 +3189,7 @@
       <c r="M87" s="8"/>
       <c r="N87" s="5"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -3211,7 +3205,7 @@
       <c r="M88" s="8"/>
       <c r="N88" s="5"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -3227,7 +3221,7 @@
       <c r="M89" s="8"/>
       <c r="N89" s="5"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -3243,7 +3237,7 @@
       <c r="M90" s="8"/>
       <c r="N90" s="5"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -3259,7 +3253,7 @@
       <c r="M91" s="8"/>
       <c r="N91" s="5"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="8"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -3275,7 +3269,7 @@
       <c r="M92" s="8"/>
       <c r="N92" s="5"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -3291,7 +3285,7 @@
       <c r="M93" s="8"/>
       <c r="N93" s="5"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="8"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -3307,7 +3301,7 @@
       <c r="M94" s="8"/>
       <c r="N94" s="5"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="8"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -3323,7 +3317,7 @@
       <c r="M95" s="8"/>
       <c r="N95" s="5"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="8"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -3339,7 +3333,7 @@
       <c r="M96" s="8"/>
       <c r="N96" s="5"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -3355,7 +3349,7 @@
       <c r="M97" s="8"/>
       <c r="N97" s="5"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -3371,7 +3365,7 @@
       <c r="M98" s="8"/>
       <c r="N98" s="5"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="8"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -3387,7 +3381,7 @@
       <c r="M99" s="8"/>
       <c r="N99" s="5"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="8"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -3403,7 +3397,7 @@
       <c r="M100" s="8"/>
       <c r="N100" s="5"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="8"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -3436,12 +3430,12 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="83.625" customWidth="1"/>
+    <col min="8" max="8" width="83.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3464,7 +3458,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3485,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3508,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3535,7 +3529,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3562,7 +3556,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3589,7 +3583,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3616,7 +3610,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3643,7 +3637,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3670,7 +3664,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3697,7 +3691,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3724,7 +3718,7 @@
         <v>6.4969873726184184E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D12" s="3">
         <f>SUM(D2:D11)</f>
         <v>3239.1749169999998</v>
@@ -3746,22 +3740,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5631C922-7396-401E-9E28-CC3C884EF152}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -3772,7 +3766,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -3783,7 +3777,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -3800,7 +3794,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -3819,7 +3813,7 @@
         <v>51.981806367771277</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -3838,7 +3832,7 @@
         <v>38.98635477582846</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -3860,7 +3854,7 @@
         <v>25.990903183885639</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -3881,7 +3875,7 @@
         <v>12.995451591942819</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -3900,7 +3894,7 @@
         <v>129.95451591942819</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -3914,7 +3908,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -3948,7 +3942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3985,7 +3979,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -4020,7 +4014,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -4055,7 +4049,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -4088,7 +4082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -4116,7 +4110,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -4127,7 +4121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -4136,7 +4130,7 @@
         <v>63.742690058479539</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -4147,7 +4141,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -4159,7 +4153,7 @@
         <v>0.27280000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -4171,7 +4165,7 @@
         <v>0.13769999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -4183,7 +4177,7 @@
         <v>6.0600000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -4192,7 +4186,7 @@
         <v>1.9400000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -4219,21 +4213,21 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F1" s="15" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -4265,7 +4259,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4304,7 +4298,7 @@
         <v>7.4079252129274551E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4343,7 +4337,7 @@
         <v>8.6425794150820314E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4382,7 +4376,7 @@
         <v>9.0709288321560666E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4421,7 +4415,7 @@
         <v>8.8895102555129463E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4460,7 +4454,7 @@
         <v>8.3250969059565696E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4499,7 +4493,7 @@
         <v>7.4381616423679751E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4538,7 +4532,7 @@
         <v>6.5764234033131486E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4577,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D11">
         <f>SUM(D3:D10)</f>
         <v>7454</v>
@@ -4596,24 +4590,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178CEE79-A0CA-4272-970B-A5A5902A61A6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.5" customWidth="1"/>
-    <col min="11" max="11" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F1" s="15" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -4648,11 +4642,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>500</v>
       </c>
       <c r="C3">
@@ -4694,7 +4688,7 @@
         <v>0.32692356102142694</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4741,7 +4735,7 @@
         <v>0.22884649271499885</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4788,7 +4782,7 @@
         <v>0.16019254490049917</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4835,7 +4829,7 @@
         <v>0.11213478143034941</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4882,7 +4876,7 @@
         <v>7.849434700124458E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4929,7 +4923,7 @@
         <v>5.4946042900871205E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4976,7 +4970,7 @@
         <v>3.8462230030609841E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -5023,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="12" t="s">
         <v>87</v>
       </c>
@@ -5040,19 +5034,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>